<commit_message>
updated new test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/apium/poc/utilities/testdata/Test_Data_new.xlsx
+++ b/src/main/java/com/apium/poc/utilities/testdata/Test_Data_new.xlsx
@@ -417,12 +417,12 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>